<commit_message>
Save image in folder Manager
Changed location of the safe image function, from Application to FolderManager.
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/data_results.xlsx
+++ b/code/results/2021_monthly_results/data_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t xml:space="preserve">Male Null(-) </t>
   </si>
@@ -25,31 +25,19 @@
     <t>mice #</t>
   </si>
   <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female Null(-) </t>
+  </si>
+  <si>
     <t>4</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female Null(-) </t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Male R403Q(+/-)</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>3</t>
   </si>
   <si>
     <t>Female R403Q(+/-)</t>
@@ -143,8 +131,8 @@
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>487690</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>182890</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>137167</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -162,7 +150,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7315200" y="0"/>
-          <a:ext cx="4754890" cy="4754890"/>
+          <a:ext cx="4754890" cy="3566167"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -459,7 +447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -475,11 +463,11 @@
       </c>
       <c r="E1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -517,44 +505,22 @@
         <v>4</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="D4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Naming the excel sheet based on the date plotted
Excel worksheets can now be added and they are adopting the name of the image plotted, which have the recorded date
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/data_results.xlsx
+++ b/code/results/2021_monthly_results/data_results.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="June" sheetId="1" r:id="rId1"/>
+    <sheet name="May" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t xml:space="preserve">Male Null(-) </t>
   </si>
@@ -25,19 +25,22 @@
     <t>mice #</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Female Null(-) </t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Male R403Q(+/-)</t>
+  </si>
+  <si>
     <t>3</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Female Null(-) </t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>Male R403Q(+/-)</t>
   </si>
   <si>
     <t>Female R403Q(+/-)</t>
@@ -467,7 +470,7 @@
       </c>
       <c r="H1" s="1"/>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1"/>
     </row>
@@ -514,13 +517,13 @@
         <v>3</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
readme file deleted to avoid mistakes in github pages
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/data_results.xlsx
+++ b/code/results/2021_monthly_results/data_results.xlsx
@@ -6,14 +6,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-131" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-29" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-131" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -187,34 +188,6 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="3810000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -239,6 +212,34 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -366,6 +367,39 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
         <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
@@ -389,7 +423,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -713,6 +747,520 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -725,7 +1273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1369,520 +1917,6 @@
       </c>
       <c r="E27" t="n">
         <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date_of_birth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E2" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E3" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E4" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E5" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E6" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E8" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E10" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E11" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E12" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E13" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E14" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E15" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E16" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E17" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E18" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E19" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E20" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E21" t="n">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1959,7 +1993,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -1982,7 +2016,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -2005,7 +2039,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -2028,7 +2062,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -2051,7 +2085,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -2074,7 +2108,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -2097,7 +2131,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -2120,7 +2154,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -2143,7 +2177,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -2166,7 +2200,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -2189,7 +2223,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -2212,7 +2246,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -2235,7 +2269,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -2258,7 +2292,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -2281,7 +2315,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -2304,7 +2338,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -2327,7 +2361,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -2350,7 +2384,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -2373,7 +2407,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -2396,7 +2430,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2473,7 +2507,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -2496,7 +2530,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -2519,7 +2553,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -2542,7 +2576,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -2565,7 +2599,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -2588,7 +2622,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -2611,7 +2645,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -2634,7 +2668,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -2657,7 +2691,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -2680,7 +2714,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -2703,7 +2737,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -2726,7 +2760,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -2749,7 +2783,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -2772,7 +2806,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -2795,7 +2829,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -2818,7 +2852,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -2841,7 +2875,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -2864,7 +2898,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -2887,7 +2921,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -2910,7 +2944,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2987,7 +3021,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -3010,7 +3044,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -3033,7 +3067,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -3056,7 +3090,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -3079,7 +3113,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -3102,7 +3136,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -3125,7 +3159,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -3148,7 +3182,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -3171,7 +3205,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -3194,7 +3228,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -3217,7 +3251,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -3240,7 +3274,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -3263,7 +3297,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -3286,7 +3320,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -3309,7 +3343,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -3332,7 +3366,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -3355,7 +3389,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -3378,7 +3412,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -3401,7 +3435,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -3424,7 +3458,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3434,6 +3468,520 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3945,7 +4493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Revert "Updates on pages"
This reverts commit 2cc322b881705fe3d51da0bd3427dd621d234bb2.
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/data_results.xlsx
+++ b/code/results/2021_monthly_results/data_results.xlsx
@@ -6,19 +6,17 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-01-04" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-15" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-21" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-29" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-31" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-29" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-311" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-31" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-29" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-131" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -27,9 +25,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -83,7 +80,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
@@ -93,7 +90,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,15 +190,13 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
   </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>7</col>
@@ -213,127 +207,17 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="3810000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="3810000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="3810000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -353,7 +237,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -363,9 +247,7 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -388,7 +270,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -398,9 +280,35 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -423,7 +331,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -433,9 +341,7 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -458,7 +364,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -468,39 +374,7 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="3810000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -523,7 +397,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -533,9 +407,7 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -558,7 +430,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -568,39 +440,7 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="3810000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -970,511 +810,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date_of_birth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E2" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E3" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E4" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E5" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E6" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E8" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E10" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E11" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D12" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E12" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E13" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D14" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E14" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D15" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E15" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D16" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E16" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D17" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E17" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D18" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E18" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D19" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E19" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D20" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E20" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D21" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E21" t="n">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1486,1028 +830,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date_of_birth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E8" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E10" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E11" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E14" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E15" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E16" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E17" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E18" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E19" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E20" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E21" t="n">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date_of_birth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E2" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E3" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E4" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E5" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E6" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E8" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E10" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E11" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E12" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E13" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E14" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E15" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E16" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E17" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E18" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E19" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E20" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E21" t="n">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -3010,7 +1334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3530,13 +1854,17 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3586,7 +1914,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -3609,7 +1937,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -3632,7 +1960,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
@@ -3655,7 +1983,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -3678,7 +2006,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -3701,7 +2029,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -3724,7 +2052,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -3747,7 +2075,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
@@ -3770,7 +2098,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -3793,7 +2121,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
@@ -3816,7 +2144,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
@@ -3839,7 +2167,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
@@ -3862,7 +2190,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
@@ -3885,7 +2213,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
@@ -3908,7 +2236,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -3931,7 +2259,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
@@ -3954,7 +2282,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
@@ -3977,7 +2305,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
@@ -4000,7 +2328,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
@@ -4023,7 +2351,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -4044,9 +2372,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4096,7 +2428,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -4119,7 +2451,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -4142,7 +2474,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -4165,7 +2497,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -4188,7 +2520,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -4211,7 +2543,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -4234,7 +2566,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -4257,7 +2589,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
@@ -4280,7 +2612,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -4303,7 +2635,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -4326,7 +2658,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
@@ -4349,7 +2681,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
@@ -4372,7 +2704,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
@@ -4395,7 +2727,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
@@ -4418,7 +2750,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">
@@ -4441,7 +2773,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18">
@@ -4464,7 +2796,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
@@ -4487,7 +2819,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20">
@@ -4510,7 +2842,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
@@ -4533,7 +2865,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4548,507 +2880,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date_of_birth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E3" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E5" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E8" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E10" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E11" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E14" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E15" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E16" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E17" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E18" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E19" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E20" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E21" t="n">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5058,15 +2898,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5116,7 +2960,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -5139,7 +2983,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -5162,7 +3006,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -5185,7 +3029,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -5208,7 +3052,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -5231,7 +3075,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -5254,7 +3098,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -5277,7 +3121,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -5300,7 +3144,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -5323,7 +3167,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -5346,7 +3190,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -5369,7 +3213,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -5392,7 +3236,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -5415,7 +3259,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -5438,7 +3282,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -5461,7 +3305,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -5484,7 +3328,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -5507,7 +3351,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -5530,7 +3374,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -5553,7 +3397,145 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>34</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E22" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E26" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D27" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -5574,9 +3556,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5626,7 +3612,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -5649,7 +3635,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -5672,7 +3658,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -5695,7 +3681,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -5718,7 +3704,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -5741,7 +3727,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -5764,7 +3750,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -5787,7 +3773,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -5810,7 +3796,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -5833,7 +3819,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -5856,7 +3842,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -5879,7 +3865,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -5902,7 +3888,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -5925,7 +3911,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -5948,7 +3934,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -5971,7 +3957,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -5994,7 +3980,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -6017,7 +4003,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -6040,7 +4026,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -6063,7 +4049,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -6078,15 +4064,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6136,7 +4126,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -6159,7 +4149,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -6182,7 +4172,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -6205,7 +4195,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -6228,7 +4218,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -6251,7 +4241,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -6274,7 +4264,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -6297,7 +4287,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -6320,7 +4310,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -6343,7 +4333,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -6366,7 +4356,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -6389,7 +4379,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -6412,7 +4402,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -6435,7 +4425,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -6458,7 +4448,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -6481,7 +4471,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -6504,7 +4494,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -6527,7 +4517,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -6550,7 +4540,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -6573,145 +4563,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D22" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E22" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D23" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E23" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D24" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E24" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D25" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E25" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D26" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E26" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D27" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E27" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6732,9 +4584,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6784,7 +4640,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -6807,7 +4663,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -6830,7 +4686,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -6853,7 +4709,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -6876,7 +4732,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -6899,7 +4755,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -6922,7 +4778,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -6945,7 +4801,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -6968,7 +4824,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -6991,7 +4847,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -7014,7 +4870,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -7037,7 +4893,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -7060,7 +4916,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -7083,7 +4939,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -7106,7 +4962,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -7129,7 +4985,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -7152,7 +5008,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -7175,7 +5031,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -7198,7 +5054,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -7221,7 +5077,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -7242,9 +5098,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -7294,7 +5154,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -7317,7 +5177,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -7340,7 +5200,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
@@ -7363,7 +5223,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -7386,7 +5246,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -7409,7 +5269,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -7432,7 +5292,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
@@ -7455,7 +5315,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -7478,7 +5338,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -7501,7 +5361,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
@@ -7524,7 +5384,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -7547,7 +5407,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
@@ -7570,7 +5430,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -7593,7 +5453,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -7616,7 +5476,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -7639,7 +5499,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
@@ -7662,7 +5522,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19">
@@ -7685,7 +5545,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -7708,7 +5568,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -7731,7 +5591,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on mice data
Ideally. the data should be extracted from RedCap. yet the code to do so is not working at the moment so I am working with the raw data instead. Hence, that's why this excel file was added.
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/data_results.xlsx
+++ b/code/results/2021_monthly_results/data_results.xlsx
@@ -6,17 +6,19 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-311" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-31" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-29" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-131" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-01-04" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-15" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-21" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-29" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-31" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-29" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -25,8 +27,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -80,7 +83,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center"/>
@@ -90,6 +93,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -190,13 +194,15 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
       </spPr>
     </pic>
     <clientData/>
   </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>7</col>
@@ -207,17 +213,127 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -237,7 +353,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -247,7 +363,9 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -270,7 +388,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -280,35 +398,9 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="3810000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -331,7 +423,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -341,7 +433,9 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -364,7 +458,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -374,7 +468,39 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -397,7 +523,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -407,7 +533,9 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -430,7 +558,7 @@
     <ext cx="3810000" cy="3810000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
@@ -440,7 +568,39 @@
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -810,15 +970,511 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -830,8 +1486,1028 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -1334,7 +3010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1854,17 +3530,13 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1914,7 +3586,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -1937,7 +3609,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
@@ -1960,7 +3632,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -1983,7 +3655,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
@@ -2006,7 +3678,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
@@ -2029,7 +3701,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -2052,7 +3724,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -2075,7 +3747,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
@@ -2098,7 +3770,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
@@ -2121,7 +3793,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -2144,7 +3816,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
@@ -2167,7 +3839,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -2190,7 +3862,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -2213,7 +3885,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
@@ -2236,7 +3908,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
@@ -2259,7 +3931,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
@@ -2282,7 +3954,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
@@ -2305,7 +3977,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
@@ -2328,7 +4000,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
@@ -2351,7 +4023,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2372,13 +4044,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2428,7 +4096,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -2451,7 +4119,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -2474,7 +4142,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -2497,7 +4165,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -2520,7 +4188,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -2543,7 +4211,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -2566,7 +4234,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -2589,7 +4257,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -2612,7 +4280,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -2635,7 +4303,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -2658,7 +4326,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -2681,7 +4349,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
@@ -2704,7 +4372,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
@@ -2727,7 +4395,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -2750,7 +4418,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -2773,7 +4441,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -2796,7 +4464,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -2819,7 +4487,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -2842,7 +4510,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
@@ -2865,7 +4533,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2880,15 +4548,507 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2898,19 +5058,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2960,7 +5116,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -2983,7 +5139,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -3006,7 +5162,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
@@ -3029,7 +5185,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -3052,7 +5208,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -3075,7 +5231,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -3098,7 +5254,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -3121,7 +5277,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
@@ -3144,7 +5300,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -3167,7 +5323,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
@@ -3190,7 +5346,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
@@ -3213,7 +5369,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
@@ -3236,7 +5392,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
@@ -3259,7 +5415,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
@@ -3282,7 +5438,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -3305,7 +5461,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
@@ -3328,7 +5484,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
@@ -3351,7 +5507,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
@@ -3374,7 +5530,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
@@ -3397,145 +5553,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D22" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E22" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D23" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E23" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D24" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E24" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D25" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E25" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D26" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E26" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D27" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E27" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3556,13 +5574,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3612,7 +5626,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
@@ -3635,7 +5649,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4">
@@ -3658,7 +5672,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
@@ -3681,7 +5695,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -3704,7 +5718,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7">
@@ -3727,7 +5741,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -3750,7 +5764,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -3773,7 +5787,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
@@ -3796,7 +5810,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11">
@@ -3819,7 +5833,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
@@ -3842,7 +5856,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
@@ -3865,7 +5879,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14">
@@ -3888,7 +5902,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15">
@@ -3911,7 +5925,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16">
@@ -3934,7 +5948,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17">
@@ -3957,7 +5971,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18">
@@ -3980,7 +5994,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19">
@@ -4003,7 +6017,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20">
@@ -4026,7 +6040,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
@@ -4049,7 +6063,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4064,19 +6078,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4126,7 +6136,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -4149,7 +6159,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -4172,7 +6182,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -4195,7 +6205,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -4218,7 +6228,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -4241,7 +6251,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -4264,7 +6274,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -4287,7 +6297,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -4310,7 +6320,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -4333,7 +6343,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -4356,7 +6366,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
@@ -4379,7 +6389,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -4402,7 +6412,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -4425,7 +6435,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -4448,7 +6458,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -4471,7 +6481,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -4494,7 +6504,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -4517,7 +6527,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -4540,7 +6550,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -4563,7 +6573,145 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E22" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D23" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E23" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D24" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E24" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D25" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E25" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D26" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E26" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D27" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E27" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4584,13 +6732,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4640,7 +6784,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -4663,7 +6807,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -4686,7 +6830,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -4709,7 +6853,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -4732,7 +6876,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -4755,7 +6899,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -4778,7 +6922,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -4801,7 +6945,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -4824,7 +6968,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -4847,7 +6991,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -4870,7 +7014,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -4893,7 +7037,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -4916,7 +7060,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -4939,7 +7083,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -4962,7 +7106,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -4985,7 +7129,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -5008,7 +7152,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -5031,7 +7175,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -5054,7 +7198,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -5077,7 +7221,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5098,13 +7242,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="1" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5154,7 +7294,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -5177,7 +7317,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -5200,7 +7340,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -5223,7 +7363,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -5246,7 +7386,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -5269,7 +7409,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -5292,7 +7432,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -5315,7 +7455,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -5338,7 +7478,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -5361,7 +7501,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -5384,7 +7524,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -5407,7 +7547,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -5430,7 +7570,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -5453,7 +7593,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -5476,7 +7616,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -5499,7 +7639,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -5522,7 +7662,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -5545,7 +7685,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -5568,7 +7708,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -5591,7 +7731,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
png addition to getting started
Better description of Run Data and Histogram Display preview tabs
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/data_results.xlsx
+++ b/code/results/2021_monthly_results/data_results.xlsx
@@ -6,19 +6,20 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-01-04" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-15" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-21" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-29" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-31" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-29" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-08-31" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-01-04" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-15" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-21" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-29" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-31" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-29" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -341,7 +342,7 @@
 </wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -366,6 +367,39 @@
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <avLst/>
         </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
@@ -478,75 +512,10 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="3810000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="3" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="3810000" cy="3810000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <avLst/>
-        </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -611,6 +580,41 @@
 </wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
 <file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -628,6 +632,36 @@
       </nvPicPr>
       <blipFill>
         <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1032,7 +1066,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -1055,7 +1089,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -1078,7 +1112,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -1101,7 +1135,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -1124,7 +1158,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -1147,7 +1181,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -1170,7 +1204,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -1193,7 +1227,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -1216,7 +1250,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -1239,7 +1273,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -1262,7 +1296,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
@@ -1285,7 +1319,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
@@ -1308,7 +1342,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
@@ -1331,7 +1365,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
@@ -1354,7 +1388,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
@@ -1377,7 +1411,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
@@ -1400,7 +1434,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -1423,7 +1457,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20">
@@ -1446,7 +1480,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
@@ -1469,7 +1503,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1542,7 +1576,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -1565,7 +1599,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -1588,7 +1622,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -1611,7 +1645,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -1634,7 +1668,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -1657,7 +1691,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -1680,7 +1714,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -1703,7 +1737,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -1726,7 +1760,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -1749,7 +1783,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -1772,7 +1806,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -1795,7 +1829,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -1818,7 +1852,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -1841,7 +1875,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -1864,7 +1898,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -1887,7 +1921,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1910,7 +1944,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1933,7 +1967,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -1956,7 +1990,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -1979,7 +2013,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2052,7 +2086,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -2075,7 +2109,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -2098,7 +2132,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -2121,7 +2155,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -2144,7 +2178,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -2167,7 +2201,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -2190,7 +2224,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -2213,7 +2247,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -2236,7 +2270,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -2259,7 +2293,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -2282,7 +2316,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -2305,7 +2339,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -2328,7 +2362,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -2351,7 +2385,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -2374,7 +2408,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -2397,7 +2431,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -2420,7 +2454,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -2443,7 +2477,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -2466,7 +2500,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -2489,7 +2523,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2512,6 +2546,516 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
+    <col width="20" customWidth="1" min="1" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
     <col width="20" customWidth="1" min="1" max="3"/>
     <col width="20" customWidth="1" style="3" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
@@ -3010,7 +3554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3530,13 +4074,17 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3582,11 +4130,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
@@ -3605,11 +4153,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
@@ -3628,11 +4176,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -3651,11 +4199,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6">
@@ -3674,11 +4222,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -3697,11 +4245,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -3720,11 +4268,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9">
@@ -3743,11 +4291,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D9" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10">
@@ -3766,11 +4314,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D10" s="4" t="n">
+      <c r="D10" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11">
@@ -3789,11 +4337,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
@@ -3812,11 +4360,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13">
@@ -3835,11 +4383,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D13" s="4" t="n">
+      <c r="D13" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14">
@@ -3858,11 +4406,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D14" s="4" t="n">
+      <c r="D14" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15">
@@ -3881,11 +4429,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D15" s="4" t="n">
+      <c r="D15" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16">
@@ -3904,11 +4452,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D16" s="4" t="n">
+      <c r="D16" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
@@ -3927,11 +4475,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D17" s="4" t="n">
+      <c r="D17" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18">
@@ -3950,11 +4498,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D18" s="4" t="n">
+      <c r="D18" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19">
@@ -3973,11 +4521,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D19" s="4" t="n">
+      <c r="D19" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20">
@@ -3996,11 +4544,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D20" s="4" t="n">
+      <c r="D20" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21">
@@ -4019,11 +4567,11 @@
           <t>Alive</t>
         </is>
       </c>
-      <c r="D21" s="4" t="n">
+      <c r="D21" s="5" t="n">
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -4040,7 +4588,7 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4096,7 +4644,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -4119,7 +4667,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
@@ -4142,7 +4690,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -4165,7 +4713,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
@@ -4188,7 +4736,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
@@ -4211,7 +4759,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -4234,7 +4782,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -4257,7 +4805,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
@@ -4280,7 +4828,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
@@ -4303,7 +4851,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12">
@@ -4326,7 +4874,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13">
@@ -4349,7 +4897,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14">
@@ -4372,7 +4920,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15">
@@ -4395,7 +4943,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16">
@@ -4418,7 +4966,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17">
@@ -4441,7 +4989,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18">
@@ -4464,7 +5012,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19">
@@ -4487,7 +5035,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
@@ -4510,7 +5058,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21">
@@ -4533,7 +5081,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -4606,7 +5154,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -4629,7 +5177,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -4652,7 +5200,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -4675,7 +5223,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -4698,7 +5246,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -4721,7 +5269,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -4744,7 +5292,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -4767,7 +5315,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -4790,7 +5338,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -4813,7 +5361,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -4836,7 +5384,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -4859,7 +5407,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
@@ -4882,7 +5430,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
@@ -4905,7 +5453,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -4928,7 +5476,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -4951,7 +5499,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -4974,7 +5522,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -4997,7 +5545,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -5020,7 +5568,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
@@ -5043,7 +5591,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -5116,7 +5664,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -5139,7 +5687,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -5162,7 +5710,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -5185,7 +5733,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -5208,7 +5756,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -5231,7 +5779,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -5254,7 +5802,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -5277,7 +5825,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -5300,7 +5848,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -5323,7 +5871,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -5346,7 +5894,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -5369,7 +5917,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -5392,7 +5940,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -5415,7 +5963,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -5438,7 +5986,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -5461,7 +6009,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -5484,7 +6032,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -5507,7 +6055,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -5530,7 +6078,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -5553,7 +6101,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -5626,7 +6174,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -5649,7 +6197,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -5672,7 +6220,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
@@ -5695,7 +6243,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -5718,7 +6266,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -5741,7 +6289,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -5764,7 +6312,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -5787,7 +6335,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
@@ -5810,7 +6358,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -5833,7 +6381,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
@@ -5856,7 +6404,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
@@ -5879,7 +6427,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
@@ -5902,7 +6450,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
@@ -5925,7 +6473,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
@@ -5948,7 +6496,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -5971,7 +6519,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
@@ -5994,7 +6542,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
@@ -6017,7 +6565,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
@@ -6040,7 +6588,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
@@ -6063,7 +6611,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -6073,6 +6621,516 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -6712,516 +7770,6 @@
       </c>
       <c r="E27" t="n">
         <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date_of_birth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E2" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E3" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E4" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E5" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E6" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E8" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E10" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E11" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E12" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E13" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E14" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E15" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E16" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E17" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E18" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E19" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E20" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E21" t="n">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -7294,7 +7842,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -7317,7 +7865,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -7340,7 +7888,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -7363,7 +7911,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -7386,7 +7934,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -7409,7 +7957,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -7432,7 +7980,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -7455,7 +8003,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -7478,7 +8026,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -7501,7 +8049,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -7524,7 +8072,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -7547,7 +8095,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -7570,7 +8118,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -7593,7 +8141,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -7616,7 +8164,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -7639,7 +8187,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -7662,7 +8210,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -7685,7 +8233,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -7708,7 +8256,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -7731,7 +8279,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding Run Application to docs pages
adding Run Application to docs pages and other minor additions to the website
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/data_results.xlsx
+++ b/code/results/2021_monthly_results/data_results.xlsx
@@ -6,20 +6,21 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-08-31" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-01-04" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-15" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-21" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-29" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-31" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-29" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-311" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-08-31" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2022-01-04" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-15" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-21" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-29" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-12-31" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-29" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-13" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-07-30" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-19" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-06-30" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-10-26" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-09-23" sheetId="15" state="visible" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -195,6 +196,9 @@
       </blipFill>
       <spPr>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:prstDash val="solid"/>
+        </a:ln>
       </spPr>
     </pic>
     <clientData/>
@@ -265,6 +269,31 @@
         <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:prstDash val="solid"/>
         </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1004,511 +1033,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="20" customWidth="1" min="5" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date_of_birth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E2" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E3" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E4" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E5" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E6" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E8" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E10" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E11" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D12" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E12" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D13" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E13" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D14" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E14" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D15" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E15" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D16" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E16" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D17" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E17" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D18" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E18" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D19" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E19" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D20" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E20" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D21" s="5" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E21" t="n">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1576,7 +1109,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -1599,7 +1132,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
@@ -1622,7 +1155,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
@@ -1645,7 +1178,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
@@ -1668,7 +1201,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
@@ -1691,7 +1224,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -1714,7 +1247,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -1737,7 +1270,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -1760,7 +1293,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -1783,7 +1316,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -1806,7 +1339,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
@@ -1829,7 +1362,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14">
@@ -1852,7 +1385,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
@@ -1875,7 +1408,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
@@ -1898,7 +1431,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
@@ -1921,7 +1454,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18">
@@ -1944,7 +1477,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
@@ -1967,7 +1500,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
@@ -1990,7 +1523,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -2013,7 +1546,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2086,7 +1619,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -2109,7 +1642,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -2132,7 +1665,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -2155,7 +1688,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -2178,7 +1711,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -2201,7 +1734,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -2224,7 +1757,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -2247,7 +1780,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -2270,7 +1803,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -2293,7 +1826,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -2316,7 +1849,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -2339,7 +1872,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -2362,7 +1895,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -2385,7 +1918,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -2408,7 +1941,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -2431,7 +1964,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -2454,7 +1987,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -2477,7 +2010,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -2500,7 +2033,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
@@ -2523,7 +2056,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2547,6 +2080,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="5"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2596,7 +2133,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -2619,7 +2156,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -2642,7 +2179,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -2665,7 +2202,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -2688,7 +2225,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -2711,7 +2248,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -2734,7 +2271,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -2757,7 +2294,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -2780,7 +2317,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -2803,7 +2340,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -2826,7 +2363,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -2849,7 +2386,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -2872,7 +2409,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -2895,7 +2432,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -2918,7 +2455,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -2941,7 +2478,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -2964,7 +2501,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -2987,7 +2524,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -3010,7 +2547,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -3033,7 +2570,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3056,6 +2593,516 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
+    <col width="20" customWidth="1" min="1" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
     <col width="20" customWidth="1" min="1" max="3"/>
     <col width="20" customWidth="1" style="3" min="4" max="4"/>
     <col width="20" customWidth="1" min="5" max="5"/>
@@ -3554,7 +3601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -4134,7 +4181,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -4157,7 +4204,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
@@ -4180,7 +4227,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -4203,7 +4250,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -4226,7 +4273,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -4249,7 +4296,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -4272,7 +4319,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -4295,7 +4342,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -4318,7 +4365,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11">
@@ -4341,7 +4388,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -4364,7 +4411,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
@@ -4387,7 +4434,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14">
@@ -4410,7 +4457,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15">
@@ -4433,7 +4480,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16">
@@ -4456,7 +4503,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17">
@@ -4479,7 +4526,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
@@ -4502,7 +4549,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -4525,7 +4572,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20">
@@ -4548,7 +4595,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
@@ -4571,7 +4618,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -4581,6 +4628,520 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="5" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -5082,516 +5643,6 @@
       </c>
       <c r="E21" t="n">
         <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date_of_birth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E3" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E4" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E5" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E6" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E8" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E10" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E11" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E12" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E13" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E14" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E15" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E16" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E17" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E18" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E19" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E20" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E21" t="n">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -5664,7 +5715,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3">
@@ -5687,7 +5738,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4">
@@ -5710,7 +5761,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5">
@@ -5733,7 +5784,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
@@ -5756,7 +5807,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -5779,7 +5830,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -5802,7 +5853,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -5825,7 +5876,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -5848,7 +5899,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -5871,7 +5922,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -5894,7 +5945,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -5917,7 +5968,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
@@ -5940,7 +5991,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
@@ -5963,7 +6014,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -5986,7 +6037,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -6009,7 +6060,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -6032,7 +6083,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -6055,7 +6106,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -6078,7 +6129,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
@@ -6101,7 +6152,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -6174,7 +6225,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -6197,7 +6248,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -6220,7 +6271,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5">
@@ -6243,7 +6294,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -6266,7 +6317,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -6289,7 +6340,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8">
@@ -6312,7 +6363,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -6335,7 +6386,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -6358,7 +6409,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -6381,7 +6432,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12">
@@ -6404,7 +6455,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -6427,7 +6478,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -6450,7 +6501,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
@@ -6473,7 +6524,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -6496,7 +6547,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17">
@@ -6519,7 +6570,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -6542,7 +6593,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -6565,7 +6616,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -6588,7 +6639,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -6611,7 +6662,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -6684,7 +6735,7 @@
         <v>44317</v>
       </c>
       <c r="E2" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -6707,7 +6758,7 @@
         <v>44317</v>
       </c>
       <c r="E3" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -6730,7 +6781,7 @@
         <v>44317</v>
       </c>
       <c r="E4" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5">
@@ -6753,7 +6804,7 @@
         <v>44317</v>
       </c>
       <c r="E5" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6">
@@ -6776,7 +6827,7 @@
         <v>44317</v>
       </c>
       <c r="E6" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -6799,7 +6850,7 @@
         <v>44317</v>
       </c>
       <c r="E7" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -6822,7 +6873,7 @@
         <v>44317</v>
       </c>
       <c r="E8" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -6845,7 +6896,7 @@
         <v>44317</v>
       </c>
       <c r="E9" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
@@ -6868,7 +6919,7 @@
         <v>44317</v>
       </c>
       <c r="E10" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -6891,7 +6942,7 @@
         <v>44317</v>
       </c>
       <c r="E11" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12">
@@ -6914,7 +6965,7 @@
         <v>44317</v>
       </c>
       <c r="E12" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
@@ -6937,7 +6988,7 @@
         <v>44317</v>
       </c>
       <c r="E13" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
@@ -6960,7 +7011,7 @@
         <v>44317</v>
       </c>
       <c r="E14" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15">
@@ -6983,7 +7034,7 @@
         <v>44317</v>
       </c>
       <c r="E15" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16">
@@ -7006,7 +7057,7 @@
         <v>44317</v>
       </c>
       <c r="E16" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17">
@@ -7029,7 +7080,7 @@
         <v>44317</v>
       </c>
       <c r="E17" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18">
@@ -7052,7 +7103,7 @@
         <v>44317</v>
       </c>
       <c r="E18" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
@@ -7075,7 +7126,7 @@
         <v>44317</v>
       </c>
       <c r="E19" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
@@ -7098,7 +7149,7 @@
         <v>44317</v>
       </c>
       <c r="E20" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
@@ -7121,7 +7172,7 @@
         <v>44317</v>
       </c>
       <c r="E21" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -7131,6 +7182,516 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="4" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -7776,514 +8337,4 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="20" customWidth="1" min="1" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Sex</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Genotype</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date_of_birth</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Calculated Age</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E2" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E3" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E4" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E5" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E6" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E7" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E8" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E9" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D10" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E10" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D11" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E11" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D12" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E12" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D13" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E13" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R403Q(+/-)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D14" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E14" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D15" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E15" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D16" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E16" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D17" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E17" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D18" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E18" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D19" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E19" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D20" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E20" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Null(-)</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Alive</t>
-        </is>
-      </c>
-      <c r="D21" s="4" t="n">
-        <v>44317</v>
-      </c>
-      <c r="E21" t="n">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated histogram display preview
</commit_message>
<xml_diff>
--- a/code/results/2021_monthly_results/data_results.xlsx
+++ b/code/results/2021_monthly_results/data_results.xlsx
@@ -1,43 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josep\Documents\GitHub\TheMiceCounter\code\results\2021_monthly_results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3385AACD-47CD-40C4-9D53-7F1AD3A6E232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="21" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2021-05-31" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -69,28 +67,121 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pandas" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Pandas" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="3810000" cy="3810000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,12 +468,532 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD58FA02-2452-4549-948F-4B3FEF30EB77}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sex</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Genotype</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_birth</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Calculated Age</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E7" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R403Q(+/-)</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E15" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E18" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E19" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E20" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Null(-)</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Alive</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>44317</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>